<commit_message>
Added entry screen from tables app
</commit_message>
<xml_diff>
--- a/app/config/tables/AccessMCH/Forms/AccessMCH/AccessMCH.xlsx
+++ b/app/config/tables/AccessMCH/Forms/AccessMCH/AccessMCH.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FB06FD-EDC8-4761-97D4-34F604C3283F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D4E691-144A-4816-9CC6-1B1995714B07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="359">
   <si>
     <t>setting_name</t>
   </si>
@@ -635,9 +635,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>assign</t>
   </si>
   <si>
     <t xml:space="preserve">Day of interview </t>
@@ -1617,22 +1614,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1652,7 +1649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1660,7 +1657,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1668,7 +1665,7 @@
         <v>25112020</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1676,7 +1673,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1688,7 +1685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1699,7 +1696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1710,7 +1707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>189</v>
       </c>
@@ -1729,34 +1726,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:P167"/>
+  <dimension ref="A1:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C125" sqref="C125"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="14" customWidth="1"/>
     <col min="4" max="4" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.26953125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="46.26953125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="29.81640625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" style="14" customWidth="1"/>
-    <col min="11" max="11" width="33.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.453125" style="14"/>
+    <col min="5" max="5" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.28515625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="46.28515625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="33.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1806,466 +1803,471 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="D3" s="12" t="s">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="I3" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
-      <c r="D4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="G4" s="25" t="s">
+      <c r="G3" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="G8" t="s">
+        <v>305</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="D13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
+      <c r="G13" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D9" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="G9" t="s">
-        <v>306</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:16" ht="87" x14ac:dyDescent="0.35">
-      <c r="D14" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>315</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B15" s="14" t="s">
-        <v>179</v>
+      <c r="C15" s="14" t="s">
+        <v>301</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+    <row r="16" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="D16" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C18" s="14" t="s">
         <v>302</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="2:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="D17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B18" s="14" t="s">
-        <v>179</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="14" t="s">
+    <row r="19" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="D19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="2:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="D20" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>319</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B21" s="14" t="s">
-        <v>179</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="18"/>
-    </row>
-    <row r="23" spans="2:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="D23" s="15" t="s">
+    <row r="22" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="D22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="G23" s="21" t="s">
+      <c r="F22" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="H22" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="H23" s="21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>179</v>
+        <v>38</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="14" t="s">
+    <row r="26" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="D26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="18"/>
-    </row>
-    <row r="27" spans="2:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="D27" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="14" t="s">
+    <row r="29" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="18"/>
-    </row>
-    <row r="30" spans="2:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="D30" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="18"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="14" t="s">
+    <row r="32" spans="2:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="D32" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="18"/>
-    </row>
-    <row r="33" spans="2:10" ht="145" x14ac:dyDescent="0.35">
-      <c r="D33" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="H33" s="21" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B34" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="18"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B35" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D36" s="15" t="s">
+    <row r="35" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="D35" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E35" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F35" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G35" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="H35" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="H36" s="21" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36"/>
+      <c r="H36" s="21"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>38</v>
+        <v>184</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>183</v>
       </c>
       <c r="E37"/>
       <c r="H37" s="21"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39"/>
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C38" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="E38"/>
-      <c r="H38" s="21"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B39" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D39" s="14"/>
-      <c r="G39" s="14"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="14" t="s">
-        <v>179</v>
+      <c r="C40" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="E40"/>
       <c r="H40" s="21"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="E41"/>
       <c r="H41" s="21"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B42" s="14" t="s">
+    <row r="42" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="H42" s="22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E42"/>
-      <c r="H42" s="21"/>
-    </row>
-    <row r="43" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="D43" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G43" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B44" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B45" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D45" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D46" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="H46" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="F46" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D47" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E47" s="21" t="s">
-        <v>208</v>
-      </c>
+      <c r="H46" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47"/>
       <c r="F47" t="s">
         <v>208</v>
       </c>
       <c r="G47" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H47" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J47" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>51</v>
       </c>
       <c r="E48"/>
       <c r="F48" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G48" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="H48" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="J48" s="14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>51</v>
       </c>
@@ -2274,1211 +2276,1193 @@
         <v>212</v>
       </c>
       <c r="G49" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H49" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D50" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50"/>
-      <c r="F50" t="s">
-        <v>213</v>
-      </c>
-      <c r="G50" t="s">
-        <v>214</v>
-      </c>
-      <c r="H50" t="s">
-        <v>214</v>
-      </c>
-      <c r="J50" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D51" s="15" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="E51" t="s">
+        <v>76</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D52" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E52" t="s">
-        <v>76</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H52" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>38</v>
+        <v>184</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="E53"/>
-      <c r="H53" s="18"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="E54"/>
       <c r="H54" s="21"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E55"/>
       <c r="H55" s="21"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="E56"/>
       <c r="H56" s="21"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>188</v>
+        <v>37</v>
       </c>
       <c r="E57"/>
       <c r="H57" s="21"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B58" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58"/>
-      <c r="H58" s="21"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D58" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G58" t="s">
+        <v>50</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D59" s="15" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G59" t="s">
-        <v>50</v>
+        <v>327</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D60" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G60" t="s">
         <v>328</v>
       </c>
-      <c r="H60" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="I60" s="18" t="s">
+      <c r="I59" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G60"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>38</v>
+        <v>179</v>
       </c>
       <c r="G61"/>
       <c r="H61" s="18"/>
       <c r="I61" s="18"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
-        <v>179</v>
+        <v>37</v>
       </c>
       <c r="G62"/>
       <c r="H62" s="18"/>
       <c r="I62" s="18"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B63" s="14" t="s">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D63" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" t="s">
+        <v>86</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D64" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="G65" s="14"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D66" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G63"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D64" s="15" t="s">
+      <c r="H69" s="18"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D70" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D71" s="14"/>
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D72" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="G72" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D76" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G64" t="s">
-        <v>86</v>
-      </c>
-      <c r="H64" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D65" s="15" t="s">
+      <c r="G76" t="s">
+        <v>84</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="G77" s="14"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D78" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D79" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E65" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="G65" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H65" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="D66" s="14"/>
-      <c r="G66" s="14"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D67" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F67" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="H67" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="14" t="s">
+      <c r="E79" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G79" s="14"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="H68" s="18"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B69" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H69" s="18"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B70" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H70" s="18"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D71" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="G71" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H71" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B72" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D72" s="14"/>
-      <c r="G72" s="14"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D73" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="H73" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B74" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="H74" s="18"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B75" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H75" s="18"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B76" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H76" s="18"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D77" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G77" t="s">
-        <v>84</v>
-      </c>
-      <c r="H77" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B78" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="G78" s="14"/>
-      <c r="H78" s="18"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D79" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G79" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="H79" s="18" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D80" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E80" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F80" s="14" t="s">
-        <v>235</v>
       </c>
       <c r="G80" s="14"/>
       <c r="H80" s="18"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>282</v>
       </c>
       <c r="G81" s="14"/>
       <c r="H81" s="18"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B82" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="14" t="s">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D82" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G82" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="G82" s="14"/>
-      <c r="H82" s="18"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H82" s="18" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D83" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G83" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="H83" s="18" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D84" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E83" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F84" s="14" t="s">
-        <v>235</v>
+      <c r="F83" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G83" s="14"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="G84" s="14"/>
       <c r="H84" s="18"/>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>285</v>
       </c>
       <c r="G85" s="14"/>
       <c r="H85" s="18"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B86" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C86" s="14" t="s">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D86" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G86" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="G86" s="14"/>
-      <c r="H86" s="18"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H86" s="18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D87" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G87" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="H87" s="18" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D88" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E88" s="14" t="s">
+      <c r="E87" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F88" s="14" t="s">
-        <v>235</v>
+      <c r="F87" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G87" s="14"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="G88" s="14"/>
       <c r="H88" s="18"/>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>288</v>
       </c>
       <c r="G89" s="14"/>
       <c r="H89" s="18"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B90" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C90" s="14" t="s">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D90" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G90" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="G90" s="14"/>
-      <c r="H90" s="18"/>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H90" s="18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D91" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G91" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="H91" s="18" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D92" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E91" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F92" s="14" t="s">
-        <v>235</v>
+      <c r="F91" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G91" s="14"/>
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="G92" s="14"/>
       <c r="H92" s="18"/>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>291</v>
       </c>
       <c r="G93" s="14"/>
       <c r="H93" s="18"/>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B94" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C94" s="14" t="s">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D94" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G94" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="G94" s="14"/>
-      <c r="H94" s="18"/>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H94" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D95" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G95" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="H95" s="18" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D96" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E96" s="14" t="s">
+      <c r="E95" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F96" s="14" t="s">
-        <v>235</v>
+      <c r="F95" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G95" s="14"/>
+      <c r="H95" s="18"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="G96" s="14"/>
       <c r="H96" s="18"/>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H97" s="18"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H98" s="18"/>
+    </row>
+    <row r="99" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D99" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="G99" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="H99" s="21" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D100" s="14"/>
+      <c r="G100" s="14"/>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D101" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G101" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H101" s="18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G97" s="14"/>
-      <c r="H97" s="18"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B98" s="14" t="s">
+      <c r="H102" s="18"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D103" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F103" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G103" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H98" s="18"/>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B99" s="14" t="s">
+      <c r="H104" s="18"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H99" s="18"/>
-    </row>
-    <row r="100" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="D100" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="E100" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F100" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="G100" s="21" t="s">
-        <v>355</v>
-      </c>
-      <c r="H100" s="21" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B101" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="D101" s="14"/>
-      <c r="G101" s="14"/>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D102" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F102" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="G102" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="H102" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B103" s="14" t="s">
+      <c r="H105" s="18"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="H106" s="18"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D107" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="H107" s="18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D108" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F108" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="H103" s="18"/>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D104" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F104" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="G104" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="H104" s="18" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B105" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H105" s="18"/>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B106" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H106" s="18"/>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B107" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="C107" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="H107" s="18"/>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D108" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="H108" s="18" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D109" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E109" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F109" s="14" t="s">
-        <v>266</v>
       </c>
       <c r="G109" s="21"/>
       <c r="H109" s="21"/>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="H110" s="18"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D111" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G111" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="H111" s="18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D112" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F112" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="G110" s="21"/>
-      <c r="H110" s="21"/>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B111" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="H111" s="18"/>
-    </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D112" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G112" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="H112" s="18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D113" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E113" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F113" s="14" t="s">
-        <v>266</v>
       </c>
       <c r="G113" s="21"/>
       <c r="H113" s="21"/>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="14" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>278</v>
       </c>
       <c r="G114" s="21"/>
       <c r="H114" s="21"/>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B115" s="14" t="s">
+    <row r="115" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D115" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F115" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G115" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H115" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="C115" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="G115" s="21"/>
-      <c r="H115" s="21"/>
-    </row>
-    <row r="116" spans="2:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="D116" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="E116" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F116" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="G116" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="H116" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="117" spans="2:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B117" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D118" s="15" t="s">
+      <c r="C116" s="14" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D117" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F118" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G118" s="18" t="s">
+      <c r="F117" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G117" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H117" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="H118" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H118" s="18"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="H119" s="18"/>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="G119" s="21"/>
+      <c r="H119" s="21"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H120" s="18"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="H121" s="18"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H122" s="18"/>
+    </row>
+    <row r="123" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D123" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E123" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F123" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G123" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H123" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D124" s="14"/>
+      <c r="G124" s="14"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D125" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F125" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="G125" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H125" s="18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G120" s="21"/>
-      <c r="H120" s="21"/>
-    </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B121" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H121" s="18"/>
-    </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B122" s="14" t="s">
+      <c r="H126" s="18"/>
+    </row>
+    <row r="127" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D127" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F127" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G127" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H127" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C122" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="H122" s="18"/>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B123" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H123" s="18"/>
-    </row>
-    <row r="124" spans="2:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="D124" s="15" t="s">
+      <c r="C128" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G128" s="21"/>
+      <c r="H128" s="21"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D129" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F129" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G129" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="H129" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D130" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E124" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F124" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="G124" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H124" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B125" s="14" t="s">
+      <c r="E130" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F130" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="G130" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H130" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C125" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="D125" s="14"/>
-      <c r="G125" s="14"/>
-    </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D126" s="15" t="s">
+      <c r="C131" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="D131" s="14"/>
+      <c r="G131" s="14"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D132" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F126" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="G126" s="18" t="s">
+      <c r="F132" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="G132" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H132" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="H126" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B127" s="14" t="s">
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="H127" s="18"/>
-    </row>
-    <row r="128" spans="2:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="D128" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E128" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F128" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="G128" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H128" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B129" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C129" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G129" s="21"/>
-      <c r="H129" s="21"/>
-    </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D130" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F130" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="G130" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="H130" s="18" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D131" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E131" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F131" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="G131" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H131" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B132" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C132" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="D132" s="14"/>
-      <c r="G132" s="14"/>
-    </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D133" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F133" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="G133" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="H133" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H133" s="18"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="14" t="s">
         <v>179</v>
       </c>
       <c r="H134" s="18"/>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H135" s="18"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="H135" s="18"/>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B136" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H136" s="18"/>
-    </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="G136" s="21"/>
+      <c r="H136" s="21"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H137" s="18"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="H138" s="18"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D139" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E139" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F139" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="G139" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H139" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G140" s="21"/>
+      <c r="H140" s="21"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D141" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F141" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G141" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="H141" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D142" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E142" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F142" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G142" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H142" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C143" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D143" s="14"/>
+      <c r="G143" s="14"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D144" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F144" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="G144" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H144" s="18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G137" s="21"/>
-      <c r="H137" s="21"/>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B138" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H138" s="18"/>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B139" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C139" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="H139" s="18"/>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D140" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E140" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F140" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="G140" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H140" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B141" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C141" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="G141" s="21"/>
-      <c r="H141" s="21"/>
-    </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D142" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F142" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G142" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="H142" s="18" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D143" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E143" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F143" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="G143" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H143" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B144" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C144" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="D144" s="14"/>
-      <c r="G144" s="14"/>
-    </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D145" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F145" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="G145" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="H145" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H145" s="18"/>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="H146" s="18"/>
-    </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B147" s="14" t="s">
+      <c r="G146" s="21"/>
+      <c r="H146" s="21"/>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D147" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E147" t="s">
+        <v>75</v>
+      </c>
+      <c r="F147" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="G147" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="H147" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C148" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E148"/>
+      <c r="G148" s="21"/>
+      <c r="H148" s="21"/>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D149" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E149" t="s">
+        <v>76</v>
+      </c>
+      <c r="F149" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="G149" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="H149" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B150" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E150"/>
+      <c r="G150" s="21"/>
+      <c r="H150" s="21"/>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D151" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="F151" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G151" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="H151" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B152" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G147" s="21"/>
-      <c r="H147" s="21"/>
-    </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D148" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E148" t="s">
-        <v>75</v>
-      </c>
-      <c r="F148" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="G148" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="H148" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B149" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C149" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="E149"/>
-      <c r="G149" s="21"/>
-      <c r="H149" s="21"/>
-    </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D150" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E150" t="s">
-        <v>76</v>
-      </c>
-      <c r="F150" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="G150" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="H150" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B151" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C151" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="E151"/>
-      <c r="G151" s="21"/>
-      <c r="H151" s="21"/>
-    </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D152" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="F152" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="G152" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="H152" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="G152" s="21"/>
+      <c r="H152" s="21"/>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" s="14" t="s">
         <v>179</v>
       </c>
       <c r="G153" s="21"/>
       <c r="H153" s="21"/>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" s="14" t="s">
         <v>179</v>
       </c>
+      <c r="E154"/>
       <c r="G154" s="21"/>
       <c r="H154" s="21"/>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H155" s="18"/>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B156" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H156" s="18"/>
+    </row>
+    <row r="157" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D157" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E157" t="s">
+        <v>75</v>
+      </c>
+      <c r="F157" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="G157" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H157" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B158" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C158" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E158"/>
+      <c r="G158" s="21"/>
+      <c r="H158" s="21"/>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D159" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F159" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="G159" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="H159" s="21" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B160" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="E155"/>
-      <c r="G155" s="21"/>
-      <c r="H155" s="21"/>
-    </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B156" s="14" t="s">
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B161" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H156" s="18"/>
-    </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B157" s="14" t="s">
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B162" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G162" s="22"/>
+      <c r="H162" s="22"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B163" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H157" s="18"/>
-    </row>
-    <row r="158" spans="2:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="D158" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E158" t="s">
-        <v>75</v>
-      </c>
-      <c r="F158" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="G158" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H158" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B159" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C159" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="E159"/>
-      <c r="G159" s="21"/>
-      <c r="H159" s="21"/>
-    </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D160" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F160" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="G160" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="H160" s="21" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B161" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B162" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B163" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G163" s="22"/>
-      <c r="H163" s="22"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A164" s="14" t="s">
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D164" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F164" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B164" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D165" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F165" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="G165" s="21" t="s">
+      <c r="G164" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="H165" s="21" t="s">
+      <c r="H164" s="21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B167" s="14" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B166" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3498,13 +3482,13 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
@@ -3512,7 +3496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
     </row>
@@ -3527,19 +3511,19 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -3553,157 +3537,157 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="12" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="12" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="12" t="str">
         <f>"5"</f>
         <v>5</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="12" t="str">
         <f>"7"</f>
         <v>7</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="12" t="str">
         <f>"8"</f>
         <v>8</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7" s="12" t="str">
         <f>"11"</f>
         <v>11</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B8" s="12" t="str">
         <f>"12"</f>
         <v>12</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="12" t="str">
         <f>"13"</f>
         <v>13</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="12" t="str">
         <f>"14"</f>
         <v>14</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B11" s="12" t="str">
         <f>"15"</f>
         <v>15</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>194</v>
       </c>
@@ -3712,13 +3696,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>194</v>
       </c>
@@ -3733,7 +3717,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>194</v>
       </c>
@@ -3748,7 +3732,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>194</v>
       </c>
@@ -3757,13 +3741,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -3778,7 +3762,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -3793,7 +3777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -3808,7 +3792,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -3823,7 +3807,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -3838,7 +3822,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -3853,7 +3837,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>88</v>
       </c>
@@ -3862,13 +3846,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>88</v>
       </c>
@@ -3877,13 +3861,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>88</v>
       </c>
@@ -3892,13 +3876,13 @@
         <v>3</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>88</v>
       </c>
@@ -3907,13 +3891,13 @@
         <v>4</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>88</v>
       </c>
@@ -3922,13 +3906,13 @@
         <v>5</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>88</v>
       </c>
@@ -3937,13 +3921,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>88</v>
       </c>
@@ -3952,13 +3936,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>352</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>88</v>
       </c>
@@ -3973,7 +3957,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>88</v>
       </c>
@@ -3988,7 +3972,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>92</v>
       </c>
@@ -4003,7 +3987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>92</v>
       </c>
@@ -4018,7 +4002,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>92</v>
       </c>
@@ -4033,7 +4017,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>92</v>
       </c>
@@ -4042,13 +4026,13 @@
         <v>4</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>92</v>
       </c>
@@ -4063,7 +4047,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>92</v>
       </c>
@@ -4078,7 +4062,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>92</v>
       </c>
@@ -4093,7 +4077,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>92</v>
       </c>
@@ -4102,13 +4086,13 @@
         <v>8</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>92</v>
       </c>
@@ -4123,7 +4107,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>92</v>
       </c>
@@ -4138,7 +4122,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>92</v>
       </c>
@@ -4153,7 +4137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>107</v>
       </c>
@@ -4169,7 +4153,7 @@
       </c>
       <c r="F42" s="14"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>107</v>
       </c>
@@ -4184,7 +4168,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>107</v>
       </c>
@@ -4199,7 +4183,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>107</v>
       </c>
@@ -4214,7 +4198,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>107</v>
       </c>
@@ -4229,7 +4213,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>107</v>
       </c>
@@ -4238,13 +4222,13 @@
         <v>6</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>107</v>
       </c>
@@ -4259,7 +4243,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>107</v>
       </c>
@@ -4274,7 +4258,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>118</v>
       </c>
@@ -4289,7 +4273,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>118</v>
       </c>
@@ -4304,7 +4288,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>118</v>
       </c>
@@ -4319,7 +4303,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>118</v>
       </c>
@@ -4334,7 +4318,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>118</v>
       </c>
@@ -4349,7 +4333,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>118</v>
       </c>
@@ -4358,13 +4342,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>118</v>
       </c>
@@ -4379,7 +4363,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>118</v>
       </c>
@@ -4394,7 +4378,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>118</v>
       </c>
@@ -4409,7 +4393,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>118</v>
       </c>
@@ -4424,7 +4408,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>118</v>
       </c>
@@ -4439,7 +4423,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>118</v>
       </c>
@@ -4454,7 +4438,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>118</v>
       </c>
@@ -4469,7 +4453,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>118</v>
       </c>
@@ -4484,7 +4468,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>118</v>
       </c>
@@ -4493,13 +4477,13 @@
         <v>15</v>
       </c>
       <c r="C64" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="D64" s="11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>118</v>
       </c>
@@ -4514,7 +4498,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>118</v>
       </c>
@@ -4529,7 +4513,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>145</v>
       </c>
@@ -4544,7 +4528,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>145</v>
       </c>
@@ -4559,7 +4543,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>145</v>
       </c>
@@ -4574,7 +4558,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>145</v>
       </c>
@@ -4589,7 +4573,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>145</v>
       </c>
@@ -4604,7 +4588,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>145</v>
       </c>
@@ -4613,13 +4597,13 @@
         <v>6</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>145</v>
       </c>
@@ -4634,7 +4618,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>145</v>
       </c>
@@ -4649,7 +4633,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>145</v>
       </c>
@@ -4658,13 +4642,13 @@
         <v>9</v>
       </c>
       <c r="C75" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="D75" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="D75" s="11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>145</v>
       </c>
@@ -4679,7 +4663,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>145</v>
       </c>
@@ -4694,7 +4678,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>145</v>
       </c>
@@ -4709,7 +4693,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>162</v>
       </c>
@@ -4718,13 +4702,13 @@
         <v>1</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>162</v>
       </c>
@@ -4739,7 +4723,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>162</v>
       </c>
@@ -4754,7 +4738,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>162</v>
       </c>
@@ -4769,7 +4753,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>164</v>
       </c>
@@ -4784,7 +4768,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>164</v>
       </c>
@@ -4799,7 +4783,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>164</v>
       </c>
@@ -4814,7 +4798,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>164</v>
       </c>
@@ -4829,7 +4813,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>164</v>
       </c>
@@ -4844,7 +4828,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>164</v>
       </c>
@@ -4853,13 +4837,13 @@
         <v>6</v>
       </c>
       <c r="C88" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D88" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="D88" s="28" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>164</v>
       </c>
@@ -4874,7 +4858,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>164</v>
       </c>
@@ -4889,286 +4873,286 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="14"/>
       <c r="B91" s="19"/>
       <c r="C91" s="29"/>
       <c r="D91" s="29"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
       <c r="B92" s="19"/>
       <c r="C92" s="29"/>
       <c r="D92" s="26"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
       <c r="B93" s="19"/>
       <c r="C93" s="29"/>
       <c r="D93" s="26"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
       <c r="B94" s="19"/>
       <c r="C94" s="16"/>
       <c r="D94" s="26"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="14"/>
       <c r="B95" s="19"/>
       <c r="C95" s="16"/>
       <c r="D95" s="26"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="B96" s="19"/>
       <c r="C96" s="26"/>
       <c r="D96" s="26"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
       <c r="B97" s="19"/>
       <c r="C97" s="16"/>
       <c r="D97" s="26"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="14"/>
       <c r="B98" s="19"/>
       <c r="C98" s="16"/>
       <c r="D98" s="26"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="14"/>
       <c r="B99" s="19"/>
       <c r="C99" s="16"/>
       <c r="D99" s="26"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="14"/>
       <c r="B100" s="19"/>
       <c r="C100" s="16"/>
       <c r="D100" s="26"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="14"/>
       <c r="B101" s="19"/>
       <c r="C101" s="16"/>
       <c r="D101" s="26"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="14"/>
       <c r="B102" s="19"/>
       <c r="C102" s="16"/>
       <c r="D102" s="26"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="14"/>
       <c r="B103" s="14"/>
       <c r="C103" s="16"/>
       <c r="D103" s="26"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
       <c r="B104" s="14"/>
       <c r="C104" s="16"/>
       <c r="D104" s="26"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
       <c r="B105" s="14"/>
       <c r="C105" s="16"/>
       <c r="D105" s="26"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="14"/>
       <c r="C106" s="16"/>
       <c r="D106" s="26"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="19"/>
       <c r="C107" s="16"/>
       <c r="D107" s="26"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
       <c r="B108" s="19"/>
       <c r="C108" s="16"/>
       <c r="D108" s="26"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="14"/>
       <c r="C109" s="16"/>
       <c r="D109" s="26"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="14"/>
       <c r="C110" s="16"/>
       <c r="D110" s="26"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="19"/>
       <c r="C111" s="16"/>
       <c r="D111" s="26"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="14"/>
       <c r="B112" s="14"/>
       <c r="C112" s="16"/>
       <c r="D112" s="26"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
       <c r="B113" s="14"/>
       <c r="C113" s="16"/>
       <c r="D113" s="26"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="14"/>
       <c r="C114" s="16"/>
       <c r="D114" s="26"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="19"/>
       <c r="C115" s="16"/>
       <c r="D115" s="26"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="14"/>
       <c r="C116" s="16"/>
       <c r="D116" s="26"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
       <c r="C117" s="16"/>
       <c r="D117" s="26"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="14"/>
       <c r="C118" s="26"/>
       <c r="D118" s="26"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="19"/>
       <c r="C119" s="16"/>
       <c r="D119" s="26"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="14"/>
       <c r="C120" s="16"/>
       <c r="D120" s="26"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="14"/>
       <c r="C121" s="16"/>
       <c r="D121" s="26"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="14"/>
       <c r="C122" s="16"/>
       <c r="D122" s="26"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="14"/>
       <c r="C123" s="16"/>
       <c r="D123" s="26"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="19"/>
       <c r="C124" s="16"/>
       <c r="D124" s="26"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
       <c r="B125" s="14"/>
       <c r="C125" s="16"/>
       <c r="D125" s="26"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
       <c r="B126" s="14"/>
       <c r="C126" s="16"/>
       <c r="D126" s="26"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
       <c r="B127" s="14"/>
       <c r="C127" s="26"/>
       <c r="D127" s="26"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
       <c r="B128" s="14"/>
       <c r="C128" s="26"/>
       <c r="D128" s="26"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="14"/>
       <c r="B129" s="19"/>
       <c r="C129" s="26"/>
       <c r="D129" s="26"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" s="7"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="7"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="7"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B135" s="7"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="7"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="7"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="7"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B139" s="7"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="7"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B141" s="7"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="7"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B143" s="7"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" s="7"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="7"/>
     </row>
   </sheetData>
@@ -5190,15 +5174,15 @@
       <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -5212,7 +5196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -5241,16 +5225,16 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>